<commit_message>
Update Excel graded exercise
</commit_message>
<xml_diff>
--- a/GradedExercise.xlsx
+++ b/GradedExercise.xlsx
@@ -186,7 +186,7 @@
     <t xml:space="preserve">No unnecessary duplication (code and templates)</t>
   </si>
   <si>
-    <t xml:space="preserve">Use of dependency injection</t>
+    <t xml:space="preserve">semantic</t>
   </si>
   <si>
     <t xml:space="preserve">Commit log (expressive commit messages, one change per commit)</t>
@@ -231,7 +231,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -262,8 +262,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,13 +291,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF18A303"/>
-        <bgColor rgb="FF339966"/>
+        <bgColor rgb="FF43C330"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF09E6F"/>
         <bgColor rgb="FFFF99CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF43C330"/>
+        <bgColor rgb="FF18A303"/>
       </patternFill>
     </fill>
   </fills>
@@ -329,7 +341,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -362,11 +374,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -450,7 +470,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF43C330"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -469,11 +489,11 @@
   </sheetPr>
   <dimension ref="B2:K49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D10" colorId="64" zoomScale="108" zoomScaleNormal="108" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G32" activeCellId="0" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.96875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.82"/>
@@ -525,11 +545,11 @@
       <c r="E4" s="2"/>
       <c r="G4" s="3" t="n">
         <f aca="false">SUM(G6:G19)</f>
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H4" s="3" t="n">
         <f aca="false">MIN(C4,G4)</f>
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -587,7 +607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="n">
         <v>2</v>
       </c>
@@ -595,7 +615,7 @@
         <v>14</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -628,7 +648,7 @@
         <v>17</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,11 +666,11 @@
       <c r="D19" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -664,32 +684,32 @@
       <c r="E21" s="2"/>
       <c r="G21" s="3" t="n">
         <f aca="false">SUM(G23:G32)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H21" s="3" t="n">
         <f aca="false">MIN(C21,G21)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E22" s="8"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D23" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="9" t="s">
         <v>21</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="9" t="s">
         <v>22</v>
       </c>
       <c r="G24" s="0" t="n">
@@ -700,11 +720,11 @@
       <c r="D25" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,7 +760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="0" t="n">
         <v>2</v>
       </c>
@@ -750,13 +770,13 @@
       <c r="G30" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K30" s="9"/>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K30" s="10"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D31" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="11" t="s">
         <v>28</v>
       </c>
       <c r="G31" s="0" t="n">
@@ -785,11 +805,11 @@
       <c r="E34" s="2"/>
       <c r="G34" s="3" t="n">
         <f aca="false">SUM(G36:G43)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H34" s="3" t="n">
         <f aca="false">MIN(C34,G34)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -803,15 +823,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D37" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="9" t="s">
         <v>32</v>
       </c>
       <c r="G37" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -881,21 +901,21 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C45" s="11" t="n">
+      <c r="C45" s="13" t="n">
         <f aca="false">SUM(C4,C21,C34)</f>
         <v>60</v>
       </c>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="12" t="n">
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="14" t="n">
         <f aca="false">SUM(H4,H21,H34)</f>
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -906,21 +926,21 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="13"/>
+      <c r="I46" s="15"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="14" t="n">
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="16" t="n">
         <f aca="false">1 + (I45 * 5 / C45)</f>
-        <v>4.33333333333333</v>
+        <v>5.58333333333333</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>